<commit_message>
Se actualizan los casos de prueba, agregando el código de error esperado en la respuesta serivicios SOAP
</commit_message>
<xml_diff>
--- a/casos-prueba-C1-2023-QA-Calidad-RF.xlsx
+++ b/casos-prueba-C1-2023-QA-Calidad-RF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DISENO11\IdeaProjects\sofka\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851F5692-B54A-4A33-BCAC-B679EAEA458F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0953BE2-5A7D-402F-9B6B-CF77FF36B037}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{40787DB2-4524-4AB5-BA72-5A97AA0B892A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{40787DB2-4524-4AB5-BA72-5A97AA0B892A}"/>
   </bookViews>
   <sheets>
     <sheet name="NumberToDollars" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="172">
   <si>
     <t>Feature</t>
   </si>
@@ -314,9 +314,6 @@
     <t>ingresa un número con espacios a la izquierda</t>
   </si>
   <si>
-    <t>retornará un mensaje de error</t>
-  </si>
-  <si>
     <t>No realizará la conversión a palabras</t>
   </si>
   <si>
@@ -663,6 +660,27 @@
   </si>
   <si>
     <t>pagar</t>
+  </si>
+  <si>
+    <t>No realizará la conversión a dólares</t>
+  </si>
+  <si>
+    <t>retornará un código de error 404</t>
+  </si>
+  <si>
+    <t>retornará un códgigo de error 404</t>
+  </si>
+  <si>
+    <t>obtendrá un código de status 200</t>
+  </si>
+  <si>
+    <t>obtendrá un código status 200</t>
+  </si>
+  <si>
+    <t>obtendrá un código status 200 ok</t>
+  </si>
+  <si>
+    <t>se retornará un código 404 de error</t>
   </si>
 </sst>
 </file>
@@ -1071,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9811EB22-81F6-4A5A-9075-00F9BF48EBD3}">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,7 +1146,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,389 +1162,405 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="C16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C33" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+      <c r="C34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C45" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
+      <c r="C46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C51" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
+      <c r="C52" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C60" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C62" t="s">
-        <v>69</v>
+      <c r="C64" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1537,10 +1571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE69E2E7-95DB-4D59-AD03-26F8BB07E70F}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,7 +1627,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1609,7 +1643,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1617,392 +1651,395 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+      <c r="C35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C46" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
+      <c r="B52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C54" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="C55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C58" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
+      <c r="C59" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C60" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="C61" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C64" t="s">
-        <v>69</v>
+      <c r="C65" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +2051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9AA2C9-5166-4C91-B3CC-BAF9E8CB8681}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
@@ -2035,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,25 +2080,25 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2069,7 +2106,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2077,18 +2114,18 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2096,7 +2133,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2104,7 +2141,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2115,26 +2152,26 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
         <v>117</v>
-      </c>
-      <c r="C18" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2179,7 @@
         <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2150,7 +2187,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,18 +2195,18 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2177,15 +2214,15 @@
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2193,7 +2230,7 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2201,7 +2238,7 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2209,18 +2246,18 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2228,7 +2265,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2236,7 +2273,7 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2244,7 +2281,7 @@
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2252,18 +2289,18 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,7 +2308,7 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2279,7 +2316,7 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2287,40 +2324,40 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2328,7 +2365,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D43" s="5">
         <v>5</v>
@@ -2345,7 +2382,7 @@
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D44" s="5">
         <v>1</v>
@@ -2378,32 +2415,32 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -2411,7 +2448,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D50" s="4">
         <v>5</v>
@@ -2425,7 +2462,7 @@
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D51" s="4">
         <v>3</v>
@@ -2445,35 +2482,35 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,16 +2518,16 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E56" s="11">
         <v>46174</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2498,10 +2535,10 @@
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E57" s="11">
         <v>45778</v>
@@ -2515,40 +2552,40 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D61" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="F61" s="7" t="s">
         <v>154</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2556,10 +2593,10 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E62" s="4">
         <v>123456789</v>
@@ -2573,10 +2610,10 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E63" s="5">
         <v>987654321</v>
@@ -2593,35 +2630,35 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D67" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E67" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="E67" s="7" t="s">
-        <v>162</v>
-      </c>
       <c r="F67" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2629,7 +2666,7 @@
         <v>15</v>
       </c>
       <c r="C68" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D68" s="12">
         <v>0.25</v>
@@ -2647,7 +2684,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D69" s="12">
         <v>0.25</v>
@@ -2665,7 +2702,7 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D70" s="12">
         <v>0.1</v>

</xml_diff>

<commit_message>
Se agrega el código status esperado en cada uno de los casos de prueba
</commit_message>
<xml_diff>
--- a/casos-prueba-C1-2023-QA-Calidad-RF.xlsx
+++ b/casos-prueba-C1-2023-QA-Calidad-RF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DISENO11\IdeaProjects\sofka\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0953BE2-5A7D-402F-9B6B-CF77FF36B037}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE5B74A-9D1D-4E04-B694-A7C6D9D82C43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{40787DB2-4524-4AB5-BA72-5A97AA0B892A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{40787DB2-4524-4AB5-BA72-5A97AA0B892A}"/>
   </bookViews>
   <sheets>
     <sheet name="NumberToDollars" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="173">
   <si>
     <t>Feature</t>
   </si>
@@ -587,9 +587,6 @@
     <t>no se redireccionará al formulario de información envío</t>
   </si>
   <si>
-    <t>completar detalles de pago con información de tarjeta inválida</t>
-  </si>
-  <si>
     <t>Se interrumpirá el proceso de compra</t>
   </si>
   <si>
@@ -681,6 +678,12 @@
   </si>
   <si>
     <t>se retornará un código 404 de error</t>
+  </si>
+  <si>
+    <t>se retornará un código de error 404</t>
+  </si>
+  <si>
+    <t>completar detalles de pago con información de tarjeta invalida</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1173,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1205,7 +1208,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,7 +1251,7 @@
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,7 +1294,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,7 +1337,7 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1342,7 +1345,7 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1385,7 +1388,7 @@
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,7 +1423,7 @@
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1428,7 +1431,7 @@
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,7 +1466,7 @@
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1471,7 +1474,7 @@
         <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1514,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,7 +1555,7 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1560,7 +1563,7 @@
         <v>15</v>
       </c>
       <c r="C64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1573,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE69E2E7-95DB-4D59-AD03-26F8BB07E70F}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1643,7 +1646,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1689,7 +1692,7 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2051,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9AA2C9-5166-4C91-B3CC-BAF9E8CB8681}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,9 +2409,15 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="D46" s="5">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5">
+        <v>1</v>
+      </c>
+      <c r="F46" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
@@ -2485,7 +2494,7 @@
         <v>109</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>122</v>
@@ -2504,13 +2513,13 @@
         <v>135</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="F55" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2521,13 +2530,13 @@
         <v>136</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E56" s="11">
         <v>46174</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2538,7 +2547,7 @@
         <v>112</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E57" s="11">
         <v>45778</v>
@@ -2552,7 +2561,7 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2560,7 +2569,7 @@
         <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>122</v>
@@ -2576,16 +2585,16 @@
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D61" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="E61" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="E61" s="7" t="s">
+      <c r="F61" s="7" t="s">
         <v>153</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2593,10 +2602,10 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E62" s="4">
         <v>123456789</v>
@@ -2610,10 +2619,10 @@
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E63" s="5">
         <v>987654321</v>
@@ -2633,7 +2642,7 @@
         <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>122</v>
@@ -2649,16 +2658,16 @@
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D67" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="E67" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="E67" s="7" t="s">
-        <v>161</v>
-      </c>
       <c r="F67" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2666,7 +2675,7 @@
         <v>15</v>
       </c>
       <c r="C68" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D68" s="12">
         <v>0.25</v>
@@ -2684,7 +2693,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D69" s="12">
         <v>0.25</v>
@@ -2702,7 +2711,7 @@
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D70" s="12">
         <v>0.1</v>

</xml_diff>